<commit_message>
automatic commenting on xlsx file
</commit_message>
<xml_diff>
--- a/herbarium label/herbarium_specimens_label_data.xlsx
+++ b/herbarium label/herbarium_specimens_label_data.xlsx
@@ -3,215 +3,396 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>jinlong</author>
+  </authors>
+  <commentList>
+    <comment ref="J6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">This species can not be found in the embedded database in herblabel package 芒箕</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Eurya (should be under, PENTAPHYLACACEAE according to The Plant List Website.)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">This species can not be found in the embedded database in herblabel package Eurya2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Eurya (should be under, PENTAPHYLACACEAE according to The Plant List Website.)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">(Empty Family) Family not accepted at The Plant List Website.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve"> ORCHIDACEAE2 (Family not accepted at The Plant List Website.) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">WARNING:STATE_PROVINCE not provided</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">WARNING:STATE_PROVINCE not provided</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">WARNING:LOCALITY not provided</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">WARNING:LOCALITY not provided</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
-  <si>
-    <t xml:space="preserve">GLOBAL_UNIQUE_IDENTIFIER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HERBARIUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLLECTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADDITIONAL_COLLECTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLLECTOR_NUMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE_COLLECTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCAL_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAMILY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPECIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTHOR_OF_SPECIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFRASPECIFIC_RANK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFRASPECIFIC_EPITHET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTHOR_OF_INFRASPECIFIC_RANK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNTRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATE_PROVINCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCALITY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGE_URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATED_INFORMATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_DEGREE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_MINUTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_SECOND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_FLAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_DEGREE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_MINUTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_SECOND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_FLAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELEVATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATTRIBUTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REMARKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEOREFERENCE_SOURCES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDENTIFIED_BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE_IDENTIFIED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPE_STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROCESSED_BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE_LASTMODIFIED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPECIMEN_LOCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kadoorie Farm and Botanic Garden Herbarium (KFBG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jinlong Zhang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JL0520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-01-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">岗柃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pentaphylacaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eurya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">groffii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Hong Kong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Territories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tai Po</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tree Planting Site of Kadoorie Farm and Botanic Garden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tree, 5m tall</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+  <si>
+    <t>GLOBAL_UNIQUE_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>HERBARIUM</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>COLLECTOR</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_COLLECTOR</t>
+  </si>
+  <si>
+    <t>COLLECTOR_NUMBER</t>
+  </si>
+  <si>
+    <t>DATE_COLLECTED</t>
+  </si>
+  <si>
+    <t>LOCAL_NAME</t>
+  </si>
+  <si>
+    <t>FAMILY</t>
+  </si>
+  <si>
+    <t>GENUS</t>
+  </si>
+  <si>
+    <t>SPECIES</t>
+  </si>
+  <si>
+    <t>AUTHOR_OF_SPECIES</t>
+  </si>
+  <si>
+    <t>INFRASPECIFIC_RANK</t>
+  </si>
+  <si>
+    <t>INFRASPECIFIC_EPITHET</t>
+  </si>
+  <si>
+    <t>AUTHOR_OF_INFRASPECIFIC_RANK</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>STATE_PROVINCE</t>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>LOCALITY</t>
+  </si>
+  <si>
+    <t>IMAGE_URL</t>
+  </si>
+  <si>
+    <t>RELATED_INFORMATION</t>
+  </si>
+  <si>
+    <t>LAT_DEGREE</t>
+  </si>
+  <si>
+    <t>LAT_MINUTE</t>
+  </si>
+  <si>
+    <t>LAT_SECOND</t>
+  </si>
+  <si>
+    <t>LAT_FLAG</t>
+  </si>
+  <si>
+    <t>LON_DEGREE</t>
+  </si>
+  <si>
+    <t>LON_MINUTE</t>
+  </si>
+  <si>
+    <t>LON_SECOND</t>
+  </si>
+  <si>
+    <t>LON_FLAG</t>
+  </si>
+  <si>
+    <t>ELEVATION</t>
+  </si>
+  <si>
+    <t>ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>REMARKS</t>
+  </si>
+  <si>
+    <t>GEOREFERENCE_SOURCES</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>IDENTIFIED_BY</t>
+  </si>
+  <si>
+    <t>DATE_IDENTIFIED</t>
+  </si>
+  <si>
+    <t>TYPE_STATUS</t>
+  </si>
+  <si>
+    <t>PROCESSED_BY</t>
+  </si>
+  <si>
+    <t>DATE_LASTMODIFIED</t>
+  </si>
+  <si>
+    <t>SPECIMEN_LOCATION</t>
+  </si>
+  <si>
+    <t>Kadoorie Farm and Botanic Garden Herbarium (KFBG)</t>
+  </si>
+  <si>
+    <t>Jinlong Zhang</t>
+  </si>
+  <si>
+    <t>JL0520</t>
+  </si>
+  <si>
+    <t>42368</t>
+  </si>
+  <si>
+    <t>岗柃</t>
+  </si>
+  <si>
+    <t>Pentaphylacaceae</t>
+  </si>
+  <si>
+    <t>Eurya</t>
+  </si>
+  <si>
+    <t>groffii</t>
+  </si>
+  <si>
+    <t>Merr.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>New Territories</t>
+  </si>
+  <si>
+    <t>Tai Po</t>
+  </si>
+  <si>
+    <t>Tree Planting Site of Kadoorie Farm and Botanic Garden</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>19.49</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>25.99</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>603</t>
+  </si>
+  <si>
+    <t>Tree, 5m tall</t>
+  </si>
+  <si>
+    <t>2016-01-18</t>
+  </si>
+  <si>
+    <t>芒箕</t>
+  </si>
+  <si>
+    <t>PENTAPHYLACACEAE</t>
+  </si>
+  <si>
+    <t>蒲公英</t>
+  </si>
+  <si>
+    <t>Asteraceae</t>
+  </si>
+  <si>
+    <t>Taraxacum</t>
+  </si>
+  <si>
+    <t>mongolicum</t>
+  </si>
+  <si>
+    <t>Hand.-Mazz.</t>
+  </si>
+  <si>
+    <t>防风</t>
+  </si>
+  <si>
+    <t>Umbelliferae</t>
+  </si>
+  <si>
+    <t>Saposhnikovia</t>
+  </si>
+  <si>
+    <t>divaricata</t>
+  </si>
+  <si>
+    <t>(Trucz.) Schischk.</t>
+  </si>
+  <si>
+    <t>Theaceae</t>
+  </si>
+  <si>
+    <t>Eurya2</t>
+  </si>
+  <si>
+    <t>Orchidaceae2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="50000" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="50001" formatCode="yyyy/mm/dd"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -219,16 +400,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -236,12 +432,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="50000" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="50001" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +767,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -641,7 +854,7 @@
       <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AK1" t="s">
@@ -670,7 +883,7 @@
       <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H2" t="s">
@@ -747,8 +960,8 @@
       <c r="AI2" t="s">
         <v>41</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>43</v>
+      <c r="AJ2" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AK2"/>
       <c r="AL2"/>
@@ -768,8 +981,8 @@
       <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" t="s">
-        <v>43</v>
+      <c r="G3" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H3" t="s">
         <v>44</v>
@@ -845,8 +1058,8 @@
       <c r="AI3" t="s">
         <v>41</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>43</v>
+      <c r="AJ3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AK3"/>
       <c r="AL3"/>
@@ -866,8 +1079,8 @@
       <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
-        <v>43</v>
+      <c r="G4" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H4" t="s">
         <v>44</v>
@@ -902,9 +1115,7 @@
       <c r="R4" t="s">
         <v>52</v>
       </c>
-      <c r="S4" t="s">
-        <v>53</v>
-      </c>
+      <c r="S4" s="1"/>
       <c r="T4"/>
       <c r="U4"/>
       <c r="V4" t="s">
@@ -943,8 +1154,8 @@
       <c r="AI4" t="s">
         <v>41</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>43</v>
+      <c r="AJ4" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AK4"/>
       <c r="AL4"/>
@@ -964,8 +1175,8 @@
       <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
-        <v>43</v>
+      <c r="G5" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H5" t="s">
         <v>44</v>
@@ -1041,8 +1252,8 @@
       <c r="AI5" t="s">
         <v>41</v>
       </c>
-      <c r="AJ5" t="s">
-        <v>43</v>
+      <c r="AJ5" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AK5"/>
       <c r="AL5"/>
@@ -1062,23 +1273,21 @@
       <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
-        <v>43</v>
+      <c r="G6" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
         <v>49</v>
@@ -1139,8 +1348,8 @@
       <c r="AI6" t="s">
         <v>41</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>43</v>
+      <c r="AJ6" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AK6"/>
       <c r="AL6"/>
@@ -1160,14 +1369,14 @@
       <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" t="s">
-        <v>43</v>
+      <c r="G7" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H7" t="s">
         <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
         <v>46</v>
@@ -1237,16 +1446,1185 @@
       <c r="AI7" t="s">
         <v>41</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>43</v>
+      <c r="AJ7" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AK7"/>
       <c r="AL7"/>
       <c r="AM7"/>
       <c r="AN7"/>
     </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8" t="s">
+        <v>54</v>
+      </c>
+      <c r="W8" t="s">
+        <v>55</v>
+      </c>
+      <c r="X8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W9" t="s">
+        <v>55</v>
+      </c>
+      <c r="X9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>51</v>
+      </c>
+      <c r="R10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10" t="s">
+        <v>54</v>
+      </c>
+      <c r="W10" t="s">
+        <v>55</v>
+      </c>
+      <c r="X10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R11" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" t="s">
+        <v>53</v>
+      </c>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11" t="s">
+        <v>54</v>
+      </c>
+      <c r="W11" t="s">
+        <v>55</v>
+      </c>
+      <c r="X11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AN11"/>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>51</v>
+      </c>
+      <c r="R12" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AN12"/>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" t="s">
+        <v>49</v>
+      </c>
+      <c r="P13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>51</v>
+      </c>
+      <c r="R13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13" t="s">
+        <v>54</v>
+      </c>
+      <c r="W13" t="s">
+        <v>55</v>
+      </c>
+      <c r="X13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AN13"/>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="1"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14" t="s">
+        <v>54</v>
+      </c>
+      <c r="W14" t="s">
+        <v>55</v>
+      </c>
+      <c r="X14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" t="s">
+        <v>53</v>
+      </c>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15" t="s">
+        <v>54</v>
+      </c>
+      <c r="W15" t="s">
+        <v>55</v>
+      </c>
+      <c r="X15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16" t="s">
+        <v>52</v>
+      </c>
+      <c r="S16" t="s">
+        <v>53</v>
+      </c>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16" t="s">
+        <v>54</v>
+      </c>
+      <c r="W16" t="s">
+        <v>55</v>
+      </c>
+      <c r="X16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" t="s">
+        <v>49</v>
+      </c>
+      <c r="P17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>51</v>
+      </c>
+      <c r="R17" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" t="s">
+        <v>53</v>
+      </c>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17" t="s">
+        <v>54</v>
+      </c>
+      <c r="W17" t="s">
+        <v>55</v>
+      </c>
+      <c r="X17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" t="s">
+        <v>49</v>
+      </c>
+      <c r="P18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>51</v>
+      </c>
+      <c r="R18"/>
+      <c r="S18" t="s">
+        <v>53</v>
+      </c>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18" t="s">
+        <v>54</v>
+      </c>
+      <c r="W18" t="s">
+        <v>55</v>
+      </c>
+      <c r="X18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" t="s">
+        <v>49</v>
+      </c>
+      <c r="O19" t="s">
+        <v>49</v>
+      </c>
+      <c r="P19" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>51</v>
+      </c>
+      <c r="R19" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19" t="s">
+        <v>53</v>
+      </c>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19" t="s">
+        <v>54</v>
+      </c>
+      <c r="W19" t="s">
+        <v>55</v>
+      </c>
+      <c r="X19" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
detecting potential date errors and geocoordinates errors
</commit_message>
<xml_diff>
--- a/herbarium label/herbarium_specimens_label_data.xlsx
+++ b/herbarium label/herbarium_specimens_label_data.xlsx
@@ -14,57 +14,9 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>jinlong</author>
+    <author>jlzhang</author>
   </authors>
   <commentList>
-    <comment ref="J13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">(should be under, PENTAPHYLACACEAE according to The Plant List Website.)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">This species can not be found in the embedded database in herblabel package Eurya2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">(should be under, PENTAPHYLACACEAE according to The Plant List Website.)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve"> ORCHIDACEAE2 (Family not accepted at The Plant List Website.) </t>
-        </r>
-      </text>
-    </comment>
     <comment ref="Q14" authorId="0" shapeId="0">
       <text>
         <r>
@@ -86,6 +38,18 @@
             <name val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">STATE_PROVINCE not provided</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">COUNTY not provided</t>
         </r>
       </text>
     </comment>
@@ -113,12 +77,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="V9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Degrees must be between 0 and 90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Longitudinal Flag must be either E or W</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -249,7 +237,7 @@
     <t>JL0520</t>
   </si>
   <si>
-    <t>42368</t>
+    <t>2015-12-30</t>
   </si>
   <si>
     <t>岗柃</t>
@@ -318,6 +306,9 @@
     <t>PENTAPHYLACACEAE</t>
   </si>
   <si>
+    <t>1905-06-14</t>
+  </si>
+  <si>
     <t>蒲公英</t>
   </si>
   <si>
@@ -333,6 +324,9 @@
     <t>Hand.-Mazz.</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
     <t>防风</t>
   </si>
   <si>
@@ -352,6 +346,12 @@
   </si>
   <si>
     <t>Eurya2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>1905-07-08</t>
   </si>
   <si>
     <t>Orchidaceae2</t>
@@ -361,11 +361,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="50000" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="50001" formatCode="yyyy/mm/dd"/>
-  </numFmts>
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -376,11 +373,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -423,11 +415,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="50000" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="50001" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,7 +730,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -827,7 +817,7 @@
       <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
       <c r="AK1" t="s">
@@ -856,7 +846,7 @@
       <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
       <c r="H2" t="s">
@@ -933,7 +923,7 @@
       <c r="AI2" t="s">
         <v>41</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" t="s">
         <v>64</v>
       </c>
       <c r="AK2"/>
@@ -954,7 +944,7 @@
       <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>64</v>
       </c>
       <c r="H3" t="s">
@@ -1031,7 +1021,7 @@
       <c r="AI3" t="s">
         <v>41</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AJ3" t="s">
         <v>64</v>
       </c>
       <c r="AK3"/>
@@ -1052,7 +1042,7 @@
       <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>64</v>
       </c>
       <c r="H4" t="s">
@@ -1127,7 +1117,7 @@
       <c r="AI4" t="s">
         <v>41</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AJ4" t="s">
         <v>64</v>
       </c>
       <c r="AK4"/>
@@ -1148,7 +1138,7 @@
       <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>64</v>
       </c>
       <c r="H5" t="s">
@@ -1225,7 +1215,7 @@
       <c r="AI5" t="s">
         <v>41</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AJ5" t="s">
         <v>64</v>
       </c>
       <c r="AK5"/>
@@ -1246,7 +1236,7 @@
       <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>64</v>
       </c>
       <c r="H6" t="s">
@@ -1323,7 +1313,7 @@
       <c r="AI6" t="s">
         <v>41</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AJ6" t="s">
         <v>64</v>
       </c>
       <c r="AK6"/>
@@ -1344,7 +1334,7 @@
       <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>64</v>
       </c>
       <c r="H7" t="s">
@@ -1421,7 +1411,7 @@
       <c r="AI7" t="s">
         <v>41</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AJ7" t="s">
         <v>64</v>
       </c>
       <c r="AK7"/>
@@ -1442,8 +1432,8 @@
       <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>64</v>
+      <c r="G8" t="s">
+        <v>66</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
@@ -1519,7 +1509,7 @@
       <c r="AI8" t="s">
         <v>41</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AJ8" t="s">
         <v>64</v>
       </c>
       <c r="AK8"/>
@@ -1540,23 +1530,23 @@
       <c r="F9" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M9" t="s">
         <v>49</v>
@@ -1581,8 +1571,8 @@
       </c>
       <c r="T9"/>
       <c r="U9"/>
-      <c r="V9" t="s">
-        <v>54</v>
+      <c r="V9" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="W9" t="s">
         <v>55</v>
@@ -1617,7 +1607,7 @@
       <c r="AI9" t="s">
         <v>41</v>
       </c>
-      <c r="AJ9" s="2" t="s">
+      <c r="AJ9" t="s">
         <v>64</v>
       </c>
       <c r="AK9"/>
@@ -1638,7 +1628,7 @@
       <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>64</v>
       </c>
       <c r="H10" t="s">
@@ -1715,7 +1705,7 @@
       <c r="AI10" t="s">
         <v>41</v>
       </c>
-      <c r="AJ10" s="2" t="s">
+      <c r="AJ10" t="s">
         <v>64</v>
       </c>
       <c r="AK10"/>
@@ -1736,23 +1726,23 @@
       <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M11" t="s">
         <v>49</v>
@@ -1813,7 +1803,7 @@
       <c r="AI11" t="s">
         <v>41</v>
       </c>
-      <c r="AJ11" s="2" t="s">
+      <c r="AJ11" t="s">
         <v>64</v>
       </c>
       <c r="AK11"/>
@@ -1834,7 +1824,7 @@
       <c r="F12" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>64</v>
       </c>
       <c r="H12" t="s">
@@ -1911,7 +1901,7 @@
       <c r="AI12" t="s">
         <v>41</v>
       </c>
-      <c r="AJ12" s="2" t="s">
+      <c r="AJ12" t="s">
         <v>64</v>
       </c>
       <c r="AK12"/>
@@ -1932,16 +1922,16 @@
       <c r="F13" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>64</v>
       </c>
       <c r="H13" t="s">
         <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
         <v>46</v>
       </c>
       <c r="K13" t="s">
@@ -2009,7 +1999,7 @@
       <c r="AI13" t="s">
         <v>41</v>
       </c>
-      <c r="AJ13" s="2" t="s">
+      <c r="AJ13" t="s">
         <v>64</v>
       </c>
       <c r="AK13"/>
@@ -2030,7 +2020,7 @@
       <c r="F14" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>64</v>
       </c>
       <c r="H14" t="s">
@@ -2103,7 +2093,7 @@
       <c r="AI14" t="s">
         <v>41</v>
       </c>
-      <c r="AJ14" s="2" t="s">
+      <c r="AJ14" t="s">
         <v>64</v>
       </c>
       <c r="AK14"/>
@@ -2124,7 +2114,7 @@
       <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>64</v>
       </c>
       <c r="H15" t="s">
@@ -2199,7 +2189,7 @@
       <c r="AI15" t="s">
         <v>41</v>
       </c>
-      <c r="AJ15" s="2" t="s">
+      <c r="AJ15" t="s">
         <v>64</v>
       </c>
       <c r="AK15"/>
@@ -2220,7 +2210,7 @@
       <c r="F16" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>64</v>
       </c>
       <c r="H16" t="s">
@@ -2229,8 +2219,8 @@
       <c r="I16" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>77</v>
+      <c r="J16" t="s">
+        <v>79</v>
       </c>
       <c r="K16" t="s">
         <v>47</v>
@@ -2282,8 +2272,8 @@
       <c r="AB16" t="s">
         <v>60</v>
       </c>
-      <c r="AC16" t="s">
-        <v>61</v>
+      <c r="AC16" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="AD16" t="s">
         <v>62</v>
@@ -2297,7 +2287,7 @@
       <c r="AI16" t="s">
         <v>41</v>
       </c>
-      <c r="AJ16" s="2" t="s">
+      <c r="AJ16" t="s">
         <v>64</v>
       </c>
       <c r="AK16"/>
@@ -2318,7 +2308,7 @@
       <c r="F17" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>64</v>
       </c>
       <c r="H17" t="s">
@@ -2395,7 +2385,7 @@
       <c r="AI17" t="s">
         <v>41</v>
       </c>
-      <c r="AJ17" s="2" t="s">
+      <c r="AJ17" t="s">
         <v>64</v>
       </c>
       <c r="AK17"/>
@@ -2449,7 +2439,7 @@
       <c r="Q18" t="s">
         <v>51</v>
       </c>
-      <c r="R18"/>
+      <c r="R18" s="1"/>
       <c r="S18" t="s">
         <v>53</v>
       </c>
@@ -2513,15 +2503,15 @@
         <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="I19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" t="s">
         <v>46</v>
       </c>
       <c r="K19" t="s">

</xml_diff>

<commit_message>
Allowing matching with Chinese Names from FRPS and FOC
</commit_message>
<xml_diff>
--- a/herbarium label/herbarium_specimens_label_data.xlsx
+++ b/herbarium label/herbarium_specimens_label_data.xlsx
@@ -41,18 +41,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="R18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">COUNTY not provided</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="S4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -89,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC16" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +85,19 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Longitudinal Flag must be either E or W</t>
+          <t xml:space="preserve">Please check the date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Please check the date</t>
         </r>
       </text>
     </comment>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -303,7 +303,19 @@
     <t>2016-01-18</t>
   </si>
   <si>
-    <t>PENTAPHYLACACEAE</t>
+    <t>防风</t>
+  </si>
+  <si>
+    <t>Umbelliferae</t>
+  </si>
+  <si>
+    <t>Saposhnikovia</t>
+  </si>
+  <si>
+    <t>divaricata</t>
+  </si>
+  <si>
+    <t>(Trucz.) Schischk.</t>
   </si>
   <si>
     <t>1905-06-14</t>
@@ -327,34 +339,67 @@
     <t>100</t>
   </si>
   <si>
-    <t>防风</t>
-  </si>
-  <si>
-    <t>Umbelliferae</t>
-  </si>
-  <si>
-    <t>Saposhnikovia</t>
-  </si>
-  <si>
-    <t>divaricata</t>
-  </si>
-  <si>
-    <t>(Trucz.) Schischk.</t>
-  </si>
-  <si>
-    <t>Theaceae</t>
-  </si>
-  <si>
-    <t>Eurya2</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>1905-07-08</t>
-  </si>
-  <si>
-    <t>Orchidaceae2</t>
+    <t>Apiaceae</t>
+  </si>
+  <si>
+    <t>短花梗黃耆</t>
+  </si>
+  <si>
+    <t>Fabaceae</t>
+  </si>
+  <si>
+    <t>Astragalus</t>
+  </si>
+  <si>
+    <t>hancockii</t>
+  </si>
+  <si>
+    <t>Bunge</t>
+  </si>
+  <si>
+    <t>香港大沙叶</t>
+  </si>
+  <si>
+    <t>Rubiaceae</t>
+  </si>
+  <si>
+    <t>Pavetta</t>
+  </si>
+  <si>
+    <t>hongkongensis</t>
+  </si>
+  <si>
+    <t>Bremek.</t>
+  </si>
+  <si>
+    <t>海刀豆</t>
+  </si>
+  <si>
+    <t>Canavalia</t>
+  </si>
+  <si>
+    <t>rosea</t>
+  </si>
+  <si>
+    <t>(Swartz) Candolle</t>
+  </si>
+  <si>
+    <t>1997-03-09</t>
+  </si>
+  <si>
+    <t>珊瑚苣苔</t>
+  </si>
+  <si>
+    <t>Gesneriaceae</t>
+  </si>
+  <si>
+    <t>Corallodiscus</t>
+  </si>
+  <si>
+    <t>cordatulus</t>
+  </si>
+  <si>
+    <t>(Craib.) Burtt.</t>
   </si>
 </sst>
 </file>
@@ -1142,19 +1187,19 @@
         <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="M5" t="s">
         <v>49</v>
@@ -1341,7 +1386,7 @@
         <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
         <v>46</v>
@@ -1432,14 +1477,14 @@
       <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="G8" t="s">
-        <v>66</v>
+      <c r="G8" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J8" t="s">
         <v>46</v>
@@ -1534,19 +1579,19 @@
         <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="M9" t="s">
         <v>49</v>
@@ -1572,7 +1617,7 @@
       <c r="T9"/>
       <c r="U9"/>
       <c r="V9" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="W9" t="s">
         <v>55</v>
@@ -1635,7 +1680,7 @@
         <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J10" t="s">
         <v>46</v>
@@ -1730,19 +1775,19 @@
         <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="K11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="M11" t="s">
         <v>49</v>
@@ -1831,7 +1876,7 @@
         <v>44</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J12" t="s">
         <v>46</v>
@@ -1926,19 +1971,19 @@
         <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="L13" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="M13" t="s">
         <v>49</v>
@@ -2027,7 +2072,7 @@
         <v>44</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J14" t="s">
         <v>46</v>
@@ -2118,19 +2163,19 @@
         <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="L15" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="M15" t="s">
         <v>49</v>
@@ -2214,19 +2259,19 @@
         <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="L16" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="M16" t="s">
         <v>49</v>
@@ -2272,8 +2317,8 @@
       <c r="AB16" t="s">
         <v>60</v>
       </c>
-      <c r="AC16" s="1" t="s">
-        <v>80</v>
+      <c r="AC16" t="s">
+        <v>61</v>
       </c>
       <c r="AD16" t="s">
         <v>62</v>
@@ -2315,7 +2360,7 @@
         <v>44</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s">
         <v>46</v>
@@ -2413,7 +2458,7 @@
         <v>44</v>
       </c>
       <c r="I18" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J18" t="s">
         <v>46</v>
@@ -2439,7 +2484,7 @@
       <c r="Q18" t="s">
         <v>51</v>
       </c>
-      <c r="R18" s="1"/>
+      <c r="R18"/>
       <c r="S18" t="s">
         <v>53</v>
       </c>
@@ -2502,23 +2547,23 @@
       <c r="F19" t="s">
         <v>42</v>
       </c>
-      <c r="G19" t="s">
-        <v>81</v>
+      <c r="G19" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="K19" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="L19" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="M19" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
checking date of collection and identification
</commit_message>
<xml_diff>
--- a/herbarium label/herbarium_specimens_label_data.xlsx
+++ b/herbarium label/herbarium_specimens_label_data.xlsx
@@ -41,6 +41,18 @@
         </r>
       </text>
     </comment>
+    <comment ref="R18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">COUNTY not provided</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="S4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -65,6 +77,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="AJ11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">WARNING:DATE_IDENTIFIED is earlier than DATE_COLLECTED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">WARNING:DATE_IDENTIFIED is earlier than DATE_COLLECTED</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="V9" authorId="0" shapeId="0">
       <text>
         <r>
@@ -77,36 +113,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Please check the date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Please check the date</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -342,6 +354,9 @@
     <t>Apiaceae</t>
   </si>
   <si>
+    <t>2014-01-18</t>
+  </si>
+  <si>
     <t>短花梗黃耆</t>
   </si>
   <si>
@@ -400,6 +415,9 @@
   </si>
   <si>
     <t>(Craib.) Burtt.</t>
+  </si>
+  <si>
+    <t>1900-01-19</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1495,7 @@
       <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>70</v>
       </c>
       <c r="H8" t="s">
@@ -1848,8 +1866,8 @@
       <c r="AI11" t="s">
         <v>41</v>
       </c>
-      <c r="AJ11" t="s">
-        <v>64</v>
+      <c r="AJ11" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="AK11"/>
       <c r="AL11"/>
@@ -1971,19 +1989,19 @@
         <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M13" t="s">
         <v>49</v>
@@ -2163,19 +2181,19 @@
         <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M15" t="s">
         <v>49</v>
@@ -2259,19 +2277,19 @@
         <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M16" t="s">
         <v>49</v>
@@ -2484,7 +2502,7 @@
       <c r="Q18" t="s">
         <v>51</v>
       </c>
-      <c r="R18"/>
+      <c r="R18" s="1"/>
       <c r="S18" t="s">
         <v>53</v>
       </c>
@@ -2547,23 +2565,23 @@
       <c r="F19" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>92</v>
+      <c r="G19" t="s">
+        <v>93</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M19" t="s">
         <v>49</v>
@@ -2624,8 +2642,8 @@
       <c r="AI19" t="s">
         <v>41</v>
       </c>
-      <c r="AJ19" t="s">
-        <v>64</v>
+      <c r="AJ19" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="AK19"/>
       <c r="AL19"/>

</xml_diff>

<commit_message>
checking of dates disabled
</commit_message>
<xml_diff>
--- a/herbarium label/herbarium_specimens_label_data.xlsx
+++ b/herbarium label/herbarium_specimens_label_data.xlsx
@@ -41,18 +41,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="R18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">COUNTY not provided</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="S4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -77,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ11" authorId="0" shapeId="0">
+    <comment ref="V9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +73,31 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">WARNING:DATE_IDENTIFIED is earlier than DATE_COLLECTED</t>
+          <t xml:space="preserve">Degrees must be between 0 and 90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Please check the date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Please check the date</t>
         </r>
       </text>
     </comment>
@@ -97,19 +109,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">WARNING:DATE_IDENTIFIED is earlier than DATE_COLLECTED</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Degrees must be between 0 and 90</t>
+          <t xml:space="preserve">Please check the date</t>
         </r>
       </text>
     </comment>
@@ -1495,7 +1495,7 @@
       <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>70</v>
       </c>
       <c r="H8" t="s">
@@ -1866,7 +1866,7 @@
       <c r="AI11" t="s">
         <v>41</v>
       </c>
-      <c r="AJ11" s="1" t="s">
+      <c r="AJ11" t="s">
         <v>78</v>
       </c>
       <c r="AK11"/>
@@ -2502,7 +2502,7 @@
       <c r="Q18" t="s">
         <v>51</v>
       </c>
-      <c r="R18" s="1"/>
+      <c r="R18"/>
       <c r="S18" t="s">
         <v>53</v>
       </c>
@@ -2565,7 +2565,7 @@
       <c r="F19" t="s">
         <v>42</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H19" t="s">

</xml_diff>